<commit_message>
73 - copy groups to all rows
</commit_message>
<xml_diff>
--- a/scripts/plan.xlsx
+++ b/scripts/plan.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chipz\Desktop\auto_schedule_backend\scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820"/>
+    <workbookView windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="37">
   <si>
     <t>Группа</t>
   </si>
@@ -35,33 +30,33 @@
     <t>181-351</t>
   </si>
   <si>
+    <t>Аудит информационной безопасности (Лекция)</t>
+  </si>
+  <si>
+    <t>Аудит информационной безопасности (Практика)</t>
+  </si>
+  <si>
+    <t>Математические основы криптологии (Лекция)</t>
+  </si>
+  <si>
+    <t>Математические основы криптологии (Практика)</t>
+  </si>
+  <si>
+    <t>История</t>
+  </si>
+  <si>
+    <t>Организация и управление службой защиты информации на предприятии (Лекция)</t>
+  </si>
+  <si>
+    <t>Организация и управление службой защиты информации на предприятии (Практика)</t>
+  </si>
+  <si>
     <t>Программирование криптографических алгоритмов</t>
   </si>
   <si>
     <t>181-352</t>
   </si>
   <si>
-    <t>Аудит информационной безопасности (Лекция)</t>
-  </si>
-  <si>
-    <t>Аудит информационной безопасности (Практика)</t>
-  </si>
-  <si>
-    <t>Математические основы криптологии (Лекция)</t>
-  </si>
-  <si>
-    <t>Математические основы криптологии (Практика)</t>
-  </si>
-  <si>
-    <t>История</t>
-  </si>
-  <si>
-    <t>Организация и управление службой защиты информации на предприятии (Лекция)</t>
-  </si>
-  <si>
-    <t>Организация и управление службой защиты информации на предприятии (Практика)</t>
-  </si>
-  <si>
     <t>181-331</t>
   </si>
   <si>
@@ -95,25 +90,25 @@
     <t>171-351</t>
   </si>
   <si>
+    <t>Безопасность жизнедеятельности (Лекция)</t>
+  </si>
+  <si>
+    <t>Безопасность жизнедеятельности (Практика)</t>
+  </si>
+  <si>
+    <t>Теория вероятнотей (Лекция)</t>
+  </si>
+  <si>
+    <t>Теория вероятнотей (Практика)</t>
+  </si>
+  <si>
+    <t>Физика (Лекция)</t>
+  </si>
+  <si>
+    <t>Физика (Практика)</t>
+  </si>
+  <si>
     <t>171-352</t>
-  </si>
-  <si>
-    <t>Безопасность жизнедеятельности (Лекция)</t>
-  </si>
-  <si>
-    <t>Безопасность жизнедеятельности (Практика)</t>
-  </si>
-  <si>
-    <t>Теория вероятнотей (Лекция)</t>
-  </si>
-  <si>
-    <t>Теория вероятнотей (Практика)</t>
-  </si>
-  <si>
-    <t>Физика (Лекция)</t>
-  </si>
-  <si>
-    <t>Физика (Практика)</t>
   </si>
   <si>
     <t>191-331</t>
@@ -137,8 +132,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,25 +150,353 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -175,9 +504,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -185,24 +756,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -326,7 +941,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -347,9 +962,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="true"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -370,7 +985,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -440,7 +1055,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -466,7 +1081,7 @@
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -489,19 +1104,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
@@ -522,63 +1137,84 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -586,66 +1222,87 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="1" t="s">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="1" t="s">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -656,45 +1313,60 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="1" t="s">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
@@ -703,8 +1375,11 @@
       </c>
     </row>
     <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -722,6 +1397,9 @@
       </c>
     </row>
     <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
@@ -730,6 +1408,9 @@
       </c>
     </row>
     <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
@@ -738,6 +1419,9 @@
       </c>
     </row>
     <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
@@ -746,6 +1430,9 @@
       </c>
     </row>
     <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
@@ -754,6 +1441,9 @@
       </c>
     </row>
     <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
@@ -773,6 +1463,9 @@
       </c>
     </row>
     <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -780,7 +1473,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
@@ -788,7 +1484,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
       </c>
@@ -796,7 +1495,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>20</v>
       </c>
@@ -804,7 +1506,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>21</v>
       </c>
@@ -817,38 +1522,50 @@
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="B40" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B41" s="1" t="s">
         <v>14</v>
       </c>
@@ -856,7 +1573,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
@@ -864,58 +1584,76 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="B48" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
@@ -924,6 +1662,9 @@
       </c>
     </row>
     <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
@@ -932,16 +1673,22 @@
       </c>
     </row>
     <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="B52" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -959,6 +1706,9 @@
       </c>
     </row>
     <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B54" s="1" t="s">
         <v>33</v>
       </c>
@@ -967,6 +1717,9 @@
       </c>
     </row>
     <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B55" s="1" t="s">
         <v>34</v>
       </c>
@@ -975,6 +1728,9 @@
       </c>
     </row>
     <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B56" s="1" t="s">
         <v>35</v>
       </c>
@@ -983,6 +1739,9 @@
       </c>
     </row>
     <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B57" s="1" t="s">
         <v>36</v>
       </c>
@@ -992,32 +1751,41 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
70 - base version of algorythm
</commit_message>
<xml_diff>
--- a/scripts/plan.xlsx
+++ b/scripts/plan.xlsx
@@ -30,28 +30,28 @@
     <t>181-351</t>
   </si>
   <si>
-    <t>Аудит информационной безопасности (Лекция)</t>
-  </si>
-  <si>
-    <t>Аудит информационной безопасности (Практика)</t>
-  </si>
-  <si>
-    <t>Математические основы криптологии (Лекция)</t>
-  </si>
-  <si>
-    <t>Математические основы криптологии (Практика)</t>
+    <t>Аудит информационной безопасности (Лекция)</t>
+  </si>
+  <si>
+    <t>Аудит информационной безопасности (Практика)</t>
+  </si>
+  <si>
+    <t>Математические основы криптологии (Лекция)</t>
+  </si>
+  <si>
+    <t>Математические основы криптологии (Практика)</t>
   </si>
   <si>
     <t>История</t>
   </si>
   <si>
-    <t>Организация и управление службой защиты информации на предприятии (Лекция)</t>
-  </si>
-  <si>
-    <t>Организация и управление службой защиты информации на предприятии (Практика)</t>
-  </si>
-  <si>
-    <t>Программирование криптографических алгоритмов</t>
+    <t>Организация и управление службой защиты информации на предприятии (Лекция)</t>
+  </si>
+  <si>
+    <t>Организация и управление службой защиты информации на предприятии (Практика)</t>
+  </si>
+  <si>
+    <t>Программирование криптографических алгоритмов (Практика)</t>
   </si>
   <si>
     <t>181-352</t>
@@ -60,25 +60,25 @@
     <t>181-331</t>
   </si>
   <si>
-    <t>Аналитика информационной безопасности</t>
+    <t>Аналитика информационной безопасности</t>
   </si>
   <si>
     <t>181-361</t>
   </si>
   <si>
-    <t>Линейная алгебра (Лекция)</t>
-  </si>
-  <si>
-    <t>Линейная алгебра (Практика)</t>
-  </si>
-  <si>
-    <t>Иностранный язык</t>
-  </si>
-  <si>
-    <t>Программирование мобильных приложений</t>
-  </si>
-  <si>
-    <t>Основы сетевых технологий</t>
+    <t>Линейная алгебра (Лекция)</t>
+  </si>
+  <si>
+    <t>Линейная алгебра (Практика)</t>
+  </si>
+  <si>
+    <t>Иностранный язык</t>
+  </si>
+  <si>
+    <t>Программирование мобильных приложений</t>
+  </si>
+  <si>
+    <t>Основы сетевых технологий</t>
   </si>
   <si>
     <t>Веб-разработка</t>
@@ -90,22 +90,22 @@
     <t>171-351</t>
   </si>
   <si>
-    <t>Безопасность жизнедеятельности (Лекция)</t>
-  </si>
-  <si>
-    <t>Безопасность жизнедеятельности (Практика)</t>
-  </si>
-  <si>
-    <t>Теория вероятнотей (Лекция)</t>
-  </si>
-  <si>
-    <t>Теория вероятнотей (Практика)</t>
-  </si>
-  <si>
-    <t>Физика (Лекция)</t>
-  </si>
-  <si>
-    <t>Физика (Практика)</t>
+    <t>Безопасность жизнедеятельности (Лекция)</t>
+  </si>
+  <si>
+    <t>Безопасность жизнедеятельности (Практика)</t>
+  </si>
+  <si>
+    <t>Теория вероятнотей (Лекция)</t>
+  </si>
+  <si>
+    <t>Теория вероятнотей (Практика)</t>
+  </si>
+  <si>
+    <t>Физика (Лекция)</t>
+  </si>
+  <si>
+    <t>Физика (Практика)</t>
   </si>
   <si>
     <t>171-352</t>
@@ -114,19 +114,19 @@
     <t>191-331</t>
   </si>
   <si>
-    <t>Работа на фрезеровочных станках</t>
-  </si>
-  <si>
-    <t>Современный дизайн (Лекция)</t>
-  </si>
-  <si>
-    <t>Современный дизайн (Практика)</t>
-  </si>
-  <si>
-    <t>История исскувств</t>
-  </si>
-  <si>
-    <t>Сопротивление материалов</t>
+    <t>Работа на фрезеровочных станках</t>
+  </si>
+  <si>
+    <t>Современный дизайн (Лекция)</t>
+  </si>
+  <si>
+    <t>Современный дизайн (Практика)</t>
+  </si>
+  <si>
+    <t>История исскувств</t>
+  </si>
+  <si>
+    <t>Сопротивление материалов</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -158,6 +158,135 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -167,136 +296,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,13 +311,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,169 +485,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,6 +502,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -524,31 +533,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,20 +555,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,153 +593,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1112,13 +1112,16 @@
   <sheetPr/>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:A57"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="6.4" style="1" customWidth="true"/>
+    <col min="2" max="2" width="65.2" style="1" customWidth="true"/>
+    <col min="3" max="3" width="12.2" style="1" customWidth="true"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>